<commit_message>
Table loads correct data
</commit_message>
<xml_diff>
--- a/PowerUppXL.xlsx
+++ b/PowerUppXL.xlsx
@@ -406,7 +406,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -439,8 +441,11 @@
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
       <c r="C3">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -461,7 +466,10 @@
         <v>9</v>
       </c>
       <c r="C6">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -482,6 +490,9 @@
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Made adjustments to date for exercise tables
</commit_message>
<xml_diff>
--- a/PowerUppXL.xlsx
+++ b/PowerUppXL.xlsx
@@ -12,7 +12,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="8090"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Squats" sheetId="4" r:id="rId1"/>
+    <sheet name="Standing_Lunges" sheetId="3" r:id="rId2"/>
+    <sheet name="Dumbbell_Curls" sheetId="2" r:id="rId3"/>
+    <sheet name="Exercise Table" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Exercise</t>
   </si>
@@ -69,13 +72,22 @@
   </si>
   <si>
     <t>Shoulder Press</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Dumbbell_Curls</t>
+  </si>
+  <si>
+    <t>Standing_Lunges</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +107,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFDC143C"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -120,10 +140,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,11 +427,123 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="5">
+        <v>43558</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="4">
+        <v>43528.925520833334</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D6">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="4">
+        <v>43528.272893518515</v>
+      </c>
+      <c r="B2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C7">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -442,17 +577,20 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>76</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4">
+      <c r="B4">
         <v>10</v>
       </c>
     </row>
@@ -465,11 +603,11 @@
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6">
-        <v>5</v>
+      <c r="B6">
+        <v>12</v>
       </c>
       <c r="D6">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -490,9 +628,6 @@
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D10">
-        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Worksheets can be loaded and added
</commit_message>
<xml_diff>
--- a/PowerUppXL.xlsx
+++ b/PowerUppXL.xlsx
@@ -12,10 +12,12 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="8090"/>
   </bookViews>
   <sheets>
-    <sheet name="Squats" sheetId="4" r:id="rId1"/>
-    <sheet name="Standing_Lunges" sheetId="3" r:id="rId2"/>
-    <sheet name="Dumbbell_Curls" sheetId="2" r:id="rId3"/>
-    <sheet name="Exercise Table" sheetId="1" r:id="rId4"/>
+    <sheet name="Sit_Ups" sheetId="6" r:id="rId1"/>
+    <sheet name="Push_Ups" sheetId="5" r:id="rId2"/>
+    <sheet name="Squats" sheetId="4" r:id="rId3"/>
+    <sheet name="Standing_Lunges" sheetId="3" r:id="rId4"/>
+    <sheet name="Dumbbell_Curls" sheetId="2" r:id="rId5"/>
+    <sheet name="Exercise Table" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>Exercise</t>
   </si>
@@ -81,6 +83,12 @@
   </si>
   <si>
     <t>Standing_Lunges</t>
+  </si>
+  <si>
+    <t>Push_Ups</t>
+  </si>
+  <si>
+    <t>Sit_Ups</t>
   </si>
 </sst>
 </file>
@@ -441,15 +449,15 @@
         <v>15</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
-        <v>43558</v>
+        <v>43559</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -460,7 +468,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -474,25 +482,20 @@
         <v>15</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="4">
-        <v>43528.925520833334</v>
+      <c r="A2" s="5">
+        <v>43559</v>
       </c>
       <c r="B2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D6">
-        <v>10</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D10">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -502,6 +505,101 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.453125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="5">
+        <v>43559</v>
+      </c>
+      <c r="B2">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C9">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="4">
+        <v>43528.925520833334</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D6">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -509,7 +607,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="15.54296875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
@@ -539,7 +637,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>

</xml_diff>

<commit_message>
DataViews are both populated with data from correct tables
</commit_message>
<xml_diff>
--- a/PowerUppXL.xlsx
+++ b/PowerUppXL.xlsx
@@ -9,15 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="8090"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="8090" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Sit_Ups" sheetId="6" r:id="rId1"/>
     <sheet name="Push_Ups" sheetId="5" r:id="rId2"/>
-    <sheet name="Squats" sheetId="4" r:id="rId3"/>
-    <sheet name="Standing_Lunges" sheetId="3" r:id="rId4"/>
-    <sheet name="Dumbbell_Curls" sheetId="2" r:id="rId5"/>
-    <sheet name="Exercise Table" sheetId="1" r:id="rId6"/>
+    <sheet name="Reverse_Leg_Lift" sheetId="9" r:id="rId3"/>
+    <sheet name="Shoulder_Press" sheetId="7" r:id="rId4"/>
+    <sheet name="Squats" sheetId="4" r:id="rId5"/>
+    <sheet name="Standing_Lunges" sheetId="3" r:id="rId6"/>
+    <sheet name="Dumbbell_Side_Bend" sheetId="8" r:id="rId7"/>
+    <sheet name="Dumbbell_Curls" sheetId="2" r:id="rId8"/>
+    <sheet name="Exercise Table" sheetId="1" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>Exercise</t>
   </si>
@@ -89,6 +92,15 @@
   </si>
   <si>
     <t>Sit_Ups</t>
+  </si>
+  <si>
+    <t>Shoulder_Press</t>
+  </si>
+  <si>
+    <t>Dumbbell_Side_Bend</t>
+  </si>
+  <si>
+    <t>Reverse_Leg_Lift</t>
   </si>
 </sst>
 </file>
@@ -437,7 +449,79 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.453125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="5">
+        <v>43566</v>
+      </c>
+      <c r="B2">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.453125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="5">
+        <v>43566</v>
+      </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -449,15 +533,15 @@
         <v>15</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
-        <v>43559</v>
+        <v>43566</v>
       </c>
       <c r="B2">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -466,36 +550,33 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
-        <v>43559</v>
+        <v>43566</v>
       </c>
       <c r="B2">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D10">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -504,18 +585,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.453125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
@@ -523,30 +606,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
-        <v>43559</v>
+        <v>43566</v>
       </c>
       <c r="B2">
         <v>12</v>
-      </c>
-      <c r="D2">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C9">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -555,11 +620,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -567,7 +634,7 @@
     <col min="2" max="2" width="14.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
@@ -575,22 +642,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
-        <v>43528.925520833334</v>
+        <v>43566</v>
       </c>
       <c r="B2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="D6">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -599,18 +656,55 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.453125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="5">
+        <v>43566</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.54296875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
@@ -618,17 +712,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
-        <v>43528.272893518515</v>
+        <v>43566</v>
       </c>
       <c r="B2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C7">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -637,7 +726,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -645,7 +734,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="17.7265625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -669,6 +758,12 @@
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B2">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
@@ -691,11 +786,17 @@
       <c r="B4">
         <v>10</v>
       </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
@@ -704,6 +805,9 @@
       <c r="B6">
         <v>12</v>
       </c>
+      <c r="C6">
+        <v>11</v>
+      </c>
       <c r="D6">
         <v>10</v>
       </c>
@@ -712,6 +816,12 @@
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>16</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
@@ -727,10 +837,16 @@
       <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="C10">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="C11">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed void Editing methods to Async methods
</commit_message>
<xml_diff>
--- a/PowerUppXL.xlsx
+++ b/PowerUppXL.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="8090" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="8090" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sit_Ups" sheetId="6" r:id="rId1"/>
@@ -624,7 +624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -644,10 +644,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
-        <v>43566</v>
+        <v>43571</v>
       </c>
       <c r="B2">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -695,7 +695,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -714,10 +714,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
-        <v>43566</v>
+        <v>43571</v>
       </c>
       <c r="B2">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -809,7 +809,7 @@
         <v>11</v>
       </c>
       <c r="D6">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -820,7 +820,7 @@
         <v>7</v>
       </c>
       <c r="D7">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Spreadsheet tables Date functioning
</commit_message>
<xml_diff>
--- a/PowerUppXL.xlsx
+++ b/PowerUppXL.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="8090" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="8090" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sit_Ups" sheetId="6" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
   <si>
     <t>Exercise</t>
   </si>
@@ -101,6 +101,15 @@
   </si>
   <si>
     <t>Reverse_Leg_Lift</t>
+  </si>
+  <si>
+    <t>22/04/2019</t>
+  </si>
+  <si>
+    <t>23/04/2019</t>
+  </si>
+  <si>
+    <t>24/04/2019</t>
   </si>
 </sst>
 </file>
@@ -447,7 +456,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -474,6 +483,14 @@
         <v>17</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -482,7 +499,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -502,11 +519,32 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="5">
-        <v>43566</v>
+      <c r="A2" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="B2">
         <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -517,7 +555,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -537,11 +575,19 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="5">
-        <v>43566</v>
+      <c r="A2" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="B2">
-        <v>9</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -587,9 +633,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -607,11 +653,19 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="5">
-        <v>43566</v>
+      <c r="A2" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="B2">
-        <v>12</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -622,9 +676,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -643,11 +697,16 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="4">
-        <v>43571</v>
+      <c r="A2" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="B2">
-        <v>20</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -679,10 +738,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
-        <v>43566</v>
+        <v>43572</v>
       </c>
       <c r="B2">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -693,10 +752,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -713,11 +772,24 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="4">
-        <v>43571</v>
+      <c r="A2" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="B2">
         <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -759,10 +831,13 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>20</v>
+        <v>99</v>
+      </c>
+      <c r="C2">
+        <v>99</v>
       </c>
       <c r="D2">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -773,10 +848,13 @@
         <v>12</v>
       </c>
       <c r="C3">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="D3">
-        <v>7</v>
+        <v>36</v>
+      </c>
+      <c r="E3">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -787,7 +865,10 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <v>9</v>
+        <v>99</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -797,6 +878,9 @@
       <c r="B5">
         <v>8</v>
       </c>
+      <c r="D5">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
@@ -809,7 +893,7 @@
         <v>11</v>
       </c>
       <c r="D6">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -819,8 +903,11 @@
       <c r="B7">
         <v>7</v>
       </c>
+      <c r="C7">
+        <v>7</v>
+      </c>
       <c r="D7">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -836,6 +923,9 @@
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="B10">
+        <v>31</v>
       </c>
       <c r="C10">
         <v>17</v>

</xml_diff>

<commit_message>
Added chart view and dynamic table label
</commit_message>
<xml_diff>
--- a/PowerUppXL.xlsx
+++ b/PowerUppXL.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="8090" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="8090" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sit_Ups" sheetId="6" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
   <si>
     <t>Exercise</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>24/04/2019</t>
+  </si>
+  <si>
+    <t>25/04/2019</t>
   </si>
 </sst>
 </file>
@@ -555,9 +558,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -588,6 +591,14 @@
       </c>
       <c r="B3">
         <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -633,9 +644,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -666,6 +677,14 @@
       </c>
       <c r="B3">
         <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -717,7 +736,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -744,6 +763,14 @@
         <v>22</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -755,7 +782,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -788,8 +815,11 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="B4">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -848,10 +878,10 @@
         <v>12</v>
       </c>
       <c r="C3">
-        <v>99</v>
+        <v>15</v>
       </c>
       <c r="D3">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="E3">
         <v>21</v>
@@ -865,7 +895,7 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>10</v>
@@ -879,7 +909,7 @@
         <v>8</v>
       </c>
       <c r="D5">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -893,7 +923,7 @@
         <v>11</v>
       </c>
       <c r="D6">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Fixed cell autoformat issue in SelectionController for EditExerciseCellAsync()
</commit_message>
<xml_diff>
--- a/PowerUppXL.xlsx
+++ b/PowerUppXL.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
   <si>
     <t>Exercise</t>
   </si>
@@ -113,6 +113,21 @@
   </si>
   <si>
     <t>25/04/2019</t>
+  </si>
+  <si>
+    <t>26/04/2019</t>
+  </si>
+  <si>
+    <t>27/04/2019</t>
+  </si>
+  <si>
+    <t>29/04/2019</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>02/05/2019</t>
   </si>
 </sst>
 </file>
@@ -172,13 +187,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -194,6 +215,219 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Graph Title</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sit_Ups!$A$1:$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Date</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4/11/2019</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24/04/2019</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sit_Ups!$A$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1797-41C5-A1A2-F4C1C2E4ADDF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="398844304"/>
+        <c:axId val="422405520"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="398844304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="422405520"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="422405520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Value</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="398844304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -459,7 +693,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -494,15 +728,24 @@
         <v>31</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -550,6 +793,14 @@
         <v>12</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -558,47 +809,127 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="10.453125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="11">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="11">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="11">
         <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="11">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="10">
+        <v>43470</v>
+      </c>
+      <c r="B7" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="10">
+        <v>43470</v>
+      </c>
+      <c r="B8" s="11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="10">
+        <v>43501</v>
+      </c>
+      <c r="B10" s="11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="5">
+        <v>43501</v>
+      </c>
+      <c r="B11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="5">
+        <v>43501</v>
+      </c>
+      <c r="B12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="5">
+        <v>43501</v>
+      </c>
+      <c r="B13">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -644,7 +975,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -687,6 +1018,14 @@
         <v>15</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -695,10 +1034,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -708,24 +1047,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="8">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B3">
-        <v>10</v>
+      <c r="A3" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="8">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="8">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="8">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="7">
+        <v>43470</v>
+      </c>
+      <c r="B6" s="8">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="7">
+        <v>43501</v>
+      </c>
+      <c r="B7" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="5">
+        <v>43501</v>
+      </c>
+      <c r="B8">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -736,7 +1118,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -771,6 +1153,14 @@
         <v>15</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -779,7 +1169,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -819,6 +1209,14 @@
         <v>26</v>
       </c>
       <c r="B4">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5">
         <v>19</v>
       </c>
     </row>
@@ -864,7 +1262,7 @@
         <v>99</v>
       </c>
       <c r="C2">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="D2">
         <v>12</v>
@@ -878,13 +1276,13 @@
         <v>12</v>
       </c>
       <c r="C3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D3">
         <v>14</v>
       </c>
       <c r="E3">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -895,10 +1293,10 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -908,6 +1306,9 @@
       <c r="B5">
         <v>8</v>
       </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
       <c r="D5">
         <v>15</v>
       </c>
@@ -934,10 +1335,10 @@
         <v>7</v>
       </c>
       <c r="C7">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D7">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
@@ -959,6 +1360,9 @@
       </c>
       <c r="C10">
         <v>17</v>
+      </c>
+      <c r="D10">
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Line chart creation and chartview added
</commit_message>
<xml_diff>
--- a/PowerUppXL.xlsx
+++ b/PowerUppXL.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="8090" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="8090" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sit_Ups" sheetId="6" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="38">
   <si>
     <t>Exercise</t>
   </si>
@@ -124,10 +124,28 @@
     <t>29/04/2019</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>02/05/2019</t>
+  </si>
+  <si>
+    <t>03/05/2019</t>
+  </si>
+  <si>
+    <t>04/05/2019</t>
+  </si>
+  <si>
+    <t>05/05/2019</t>
+  </si>
+  <si>
+    <t>06/05/2019</t>
+  </si>
+  <si>
+    <t>07/05/2019</t>
+  </si>
+  <si>
+    <t>08/05/2019</t>
+  </si>
+  <si>
+    <t>09/05/2019</t>
   </si>
 </sst>
 </file>
@@ -260,17 +278,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sit_Ups!$A$1:$A$3</c:f>
+              <c:f>Sit_Ups!$B$1</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Date</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4/11/2019</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>24/04/2019</c:v>
+                  <c:v>Sit_Ups</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -278,14 +290,37 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sit_Ups!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4/11/2019</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24/04/2019</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29/04/2019</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sit_Ups!$A$4</c:f>
+              <c:f>Sit_Ups!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -293,7 +328,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-1797-41C5-A1A2-F4C1C2E4ADDF}"/>
+              <c16:uniqueId val="{00000000-30E2-46C0-9ED2-6DD3B11CB11B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -306,11 +341,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="398844304"/>
-        <c:axId val="422405520"/>
+        <c:axId val="262144456"/>
+        <c:axId val="376367264"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="398844304"/>
+        <c:axId val="262144456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -334,10 +369,11 @@
           </c:tx>
           <c:overlay val="0"/>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="422405520"/>
+        <c:crossAx val="376367264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -345,7 +381,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="422405520"/>
+        <c:axId val="376367264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -374,7 +410,399 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="398844304"/>
+        <c:crossAx val="262144456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>&lt;Exercise&gt; Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Dumbbell_Side_Bend!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dumbbell_Side_Bend</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Dumbbell_Side_Bend!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4/17/2019</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25/04/2019</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>02/05/2019</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Dumbbell_Side_Bend!$B$2:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-86C4-4EBC-886A-F621B7F23548}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="395617016"/>
+        <c:axId val="395618000"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="395617016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Date</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="395618000"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="395618000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Reps</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="395617016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>&lt;Exercise&gt; Chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Dumbbell_Curls!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dumbbell_Curls</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Dumbbell_Curls!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>23/04/2019</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23/04/2019</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25/04/2019</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Dumbbell_Curls!$B$2:$B$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7417-46DE-AB00-7D5376134AED}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="387222608"/>
+        <c:axId val="388607504"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="387222608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Date</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="388607504"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="388607504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Reps</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="387222608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -409,6 +837,76 @@
       <xdr:colOff>184150</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>336550</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -693,10 +1191,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -736,6 +1234,22 @@
         <v>15</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -745,10 +1259,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -773,8 +1287,11 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="B3">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -782,23 +1299,55 @@
         <v>25</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B5">
-        <v>12</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>28</v>
+      <c r="A6" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="B6">
-        <v>67</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -809,10 +1358,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -869,67 +1418,35 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="10">
-        <v>43470</v>
-      </c>
-      <c r="B7" s="11">
-        <v>12</v>
+      <c r="A7" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7">
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="10">
-        <v>43470</v>
-      </c>
-      <c r="B8" s="11">
-        <v>14</v>
+      <c r="A8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8">
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="11">
-        <v>12</v>
+      <c r="A9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9">
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="10">
-        <v>43501</v>
-      </c>
-      <c r="B10" s="11">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="5">
-        <v>43501</v>
-      </c>
-      <c r="B11">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="5">
-        <v>43501</v>
-      </c>
-      <c r="B12">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="5">
-        <v>43501</v>
-      </c>
-      <c r="B13">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14">
-        <v>17</v>
+      <c r="A10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -940,45 +1457,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="5">
-        <v>43566</v>
-      </c>
-      <c r="B2">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -991,6 +1473,49 @@
         <v>15</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="5">
+        <v>43566</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.453125" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1024,6 +1549,54 @@
       </c>
       <c r="B5">
         <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1037,7 +1610,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B8" sqref="A6:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1087,28 +1660,13 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="7">
-        <v>43470</v>
-      </c>
-      <c r="B6" s="8">
-        <v>38</v>
-      </c>
+      <c r="A6"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="7">
-        <v>43501</v>
-      </c>
-      <c r="B7" s="8">
-        <v>14</v>
-      </c>
+      <c r="A7"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="5">
-        <v>43501</v>
-      </c>
-      <c r="B8">
-        <v>12</v>
-      </c>
+      <c r="A8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1118,7 +1676,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -1155,21 +1713,46 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -1220,9 +1803,26 @@
         <v>19</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1259,13 +1859,13 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>99</v>
+        <v>45</v>
       </c>
       <c r="C2">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D2">
-        <v>12</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1276,10 +1876,10 @@
         <v>12</v>
       </c>
       <c r="C3">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D3">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="E3">
         <v>15</v>
@@ -1293,10 +1893,10 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D4">
-        <v>22</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1307,7 +1907,7 @@
         <v>8</v>
       </c>
       <c r="C5">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="D5">
         <v>15</v>
@@ -1318,13 +1918,13 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C6">
         <v>11</v>
       </c>
       <c r="D6">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
@@ -1359,7 +1959,7 @@
         <v>31</v>
       </c>
       <c r="C10">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D10">
         <v>15</v>
@@ -1370,7 +1970,7 @@
         <v>14</v>
       </c>
       <c r="C11">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated how data is presented in all worksheets
</commit_message>
<xml_diff>
--- a/PowerUppXL.xlsx
+++ b/PowerUppXL.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="8090" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="8090" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sit_Ups" sheetId="6" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="33">
   <si>
     <t>Exercise</t>
   </si>
@@ -43,12 +43,6 @@
     <t>2 Sets</t>
   </si>
   <si>
-    <t>1 Set (Default)</t>
-  </si>
-  <si>
-    <t>Misc</t>
-  </si>
-  <si>
     <t>Push Ups</t>
   </si>
   <si>
@@ -67,12 +61,6 @@
     <t>Standing Lunges</t>
   </si>
   <si>
-    <t>Boxing</t>
-  </si>
-  <si>
-    <t>Just Dance</t>
-  </si>
-  <si>
     <t>Sit Ups</t>
   </si>
   <si>
@@ -88,21 +76,12 @@
     <t>Standing_Lunges</t>
   </si>
   <si>
-    <t>Push_Ups</t>
-  </si>
-  <si>
     <t>Sit_Ups</t>
   </si>
   <si>
     <t>Shoulder_Press</t>
   </si>
   <si>
-    <t>Dumbbell_Side_Bend</t>
-  </si>
-  <si>
-    <t>Reverse_Leg_Lift</t>
-  </si>
-  <si>
     <t>22/04/2019</t>
   </si>
   <si>
@@ -146,6 +125,12 @@
   </si>
   <si>
     <t>09/05/2019</t>
+  </si>
+  <si>
+    <t>13/05/2019</t>
+  </si>
+  <si>
+    <t>1 Set</t>
   </si>
 </sst>
 </file>
@@ -478,7 +463,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Dumbbell_Side_Bend</c:v>
+                  <c:v>3 Sets</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1204,10 +1189,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -1220,7 +1205,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>31</v>
@@ -1228,7 +1213,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B4">
         <v>15</v>
@@ -1236,7 +1221,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B5">
         <v>12</v>
@@ -1244,7 +1229,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -1259,9 +1244,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
@@ -1270,84 +1255,104 @@
     <col min="1" max="1" width="10.453125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="B2">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B5">
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B7">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B8">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B9">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B10">
-        <v>30</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>16</v>
+      </c>
+      <c r="D11">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1358,9 +1363,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -1369,84 +1374,101 @@
     <col min="1" max="1" width="10.453125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B2" s="11">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B3" s="11">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B4" s="11">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B5" s="11">
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B6" s="11">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B8">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B9">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B10">
         <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1470,10 +1492,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -1486,7 +1508,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B3">
         <v>15</v>
@@ -1500,10 +1522,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="Y4" sqref="Y4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1511,91 +1533,113 @@
     <col min="1" max="1" width="10.453125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B5">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B6">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B7">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B8">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B9">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B10">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13">
         <v>6</v>
       </c>
     </row>
@@ -1621,15 +1665,15 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B2" s="8">
         <v>7</v>
@@ -1637,7 +1681,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B3" s="8">
         <v>19</v>
@@ -1645,7 +1689,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B4" s="8">
         <v>44</v>
@@ -1653,7 +1697,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B5" s="8">
         <v>45</v>
@@ -1676,7 +1720,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -1687,15 +1731,21 @@
     <col min="1" max="1" width="10.453125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>43572</v>
       </c>
@@ -1703,44 +1753,52 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B3">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B4">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B7">
         <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1752,7 +1810,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -1765,15 +1823,15 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>12</v>
@@ -1781,7 +1839,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>15</v>
@@ -1789,7 +1847,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>19</v>
@@ -1797,7 +1855,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B5">
         <v>19</v>
@@ -1805,7 +1863,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B6">
         <v>14</v>
@@ -1813,10 +1871,18 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B7">
         <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1828,16 +1894,20 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1848,77 +1918,71 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>16</v>
+      </c>
+      <c r="D2">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>45</v>
-      </c>
-      <c r="C2">
-        <v>64</v>
-      </c>
-      <c r="D2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="B3">
         <v>12</v>
       </c>
       <c r="C3">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D3">
         <v>6</v>
       </c>
-      <c r="E3">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
         <v>7</v>
       </c>
-      <c r="B4">
-        <v>10</v>
-      </c>
       <c r="C4">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D4">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>8</v>
       </c>
       <c r="C5">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="D5">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="C6">
         <v>11</v>
@@ -1927,9 +1991,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>7</v>
@@ -1941,35 +2005,25 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>31</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10">
-        <v>31</v>
-      </c>
-      <c r="C10">
         <v>10</v>
       </c>
-      <c r="D10">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11">
+      <c r="C9">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added menu bar, icon and new button events
</commit_message>
<xml_diff>
--- a/PowerUppXL.xlsx
+++ b/PowerUppXL.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="8090" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="8090" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sit_Ups" sheetId="6" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="36">
   <si>
     <t>Exercise</t>
   </si>
@@ -134,6 +134,12 @@
   </si>
   <si>
     <t>14/05/2019</t>
+  </si>
+  <si>
+    <t>16/05/2019</t>
+  </si>
+  <si>
+    <t>23/05/2019</t>
   </si>
 </sst>
 </file>
@@ -449,6 +455,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -551,6 +558,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -588,6 +596,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -601,6 +610,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1247,9 +1257,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1356,6 +1366,22 @@
         <v>45</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1364,9 +1390,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
@@ -1470,6 +1496,14 @@
       </c>
       <c r="D11">
         <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1721,7 +1755,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -1800,6 +1834,14 @@
       </c>
       <c r="C8">
         <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1927,13 +1969,13 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>65</v>
       </c>
       <c r="D2">
-        <v>45</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -1958,7 +2000,7 @@
         <v>7</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D4">
         <v>9</v>
@@ -1972,7 +2014,7 @@
         <v>8</v>
       </c>
       <c r="C5">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="D5">
         <v>15</v>

</xml_diff>

<commit_message>
Added Watermark image to text box
</commit_message>
<xml_diff>
--- a/PowerUppXL.xlsx
+++ b/PowerUppXL.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="38">
   <si>
     <t>Exercise</t>
   </si>
@@ -140,6 +140,12 @@
   </si>
   <si>
     <t>23/05/2019</t>
+  </si>
+  <si>
+    <t>27/05/2019</t>
+  </si>
+  <si>
+    <t>28/05/2019</t>
   </si>
 </sst>
 </file>
@@ -455,7 +461,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -558,7 +563,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -596,7 +600,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -610,7 +613,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1390,7 +1392,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
@@ -1504,6 +1506,22 @@
       </c>
       <c r="C12">
         <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2000,7 +2018,7 @@
         <v>7</v>
       </c>
       <c r="C4">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="D4">
         <v>9</v>

</xml_diff>

<commit_message>
Added "About" message box
</commit_message>
<xml_diff>
--- a/PowerUppXL.xlsx
+++ b/PowerUppXL.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="37">
   <si>
     <t>Exercise</t>
   </si>
@@ -70,12 +70,6 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Dumbbell_Curls</t>
-  </si>
-  <si>
-    <t>Standing_Lunges</t>
-  </si>
-  <si>
     <t>Sit_Ups</t>
   </si>
   <si>
@@ -146,6 +140,9 @@
   </si>
   <si>
     <t>28/05/2019</t>
+  </si>
+  <si>
+    <t>29/05/2019</t>
   </si>
 </sst>
 </file>
@@ -657,6 +654,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -674,7 +672,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Dumbbell_Curls</c:v>
+                  <c:v>3 Sets</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -759,6 +757,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -796,6 +795,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -809,6 +809,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1207,7 +1208,7 @@
         <v>11</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -1220,7 +1221,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>31</v>
@@ -1228,7 +1229,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B4">
         <v>15</v>
@@ -1236,7 +1237,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B5">
         <v>12</v>
@@ -1244,7 +1245,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -1281,12 +1282,12 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>12</v>
@@ -1294,7 +1295,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B3">
         <v>67</v>
@@ -1302,7 +1303,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4">
         <v>15</v>
@@ -1310,7 +1311,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>33</v>
@@ -1318,7 +1319,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>64</v>
@@ -1326,7 +1327,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B7">
         <v>45</v>
@@ -1334,7 +1335,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B8">
         <v>35</v>
@@ -1342,7 +1343,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -1356,7 +1357,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -1370,7 +1371,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D11">
         <v>90</v>
@@ -1378,7 +1379,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B12">
         <v>10</v>
@@ -1392,7 +1393,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E21" sqref="E21"/>
@@ -1414,12 +1415,12 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" s="11">
         <v>18</v>
@@ -1427,7 +1428,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" s="11">
         <v>10</v>
@@ -1435,7 +1436,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" s="11">
         <v>5</v>
@@ -1443,7 +1444,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" s="11">
         <v>64</v>
@@ -1451,7 +1452,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" s="11">
         <v>12</v>
@@ -1459,7 +1460,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7">
         <v>17</v>
@@ -1467,7 +1468,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8">
         <v>35</v>
@@ -1475,7 +1476,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B9">
         <v>15</v>
@@ -1483,7 +1484,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10">
         <v>53</v>
@@ -1491,7 +1492,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11">
         <v>7</v>
@@ -1502,7 +1503,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C12">
         <v>23</v>
@@ -1510,7 +1511,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C13">
         <v>24</v>
@@ -1518,10 +1519,21 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C14">
         <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1548,7 +1560,7 @@
         <v>11</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -1561,7 +1573,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <v>15</v>
@@ -1597,12 +1609,12 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2">
         <v>21</v>
@@ -1610,7 +1622,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <v>36</v>
@@ -1618,7 +1630,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>15</v>
@@ -1626,7 +1638,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5">
         <v>17</v>
@@ -1634,7 +1646,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6">
         <v>14</v>
@@ -1642,7 +1654,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>24</v>
@@ -1650,7 +1662,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8">
         <v>12</v>
@@ -1658,7 +1670,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9">
         <v>15</v>
@@ -1666,7 +1678,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B10">
         <v>14</v>
@@ -1674,7 +1686,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B11">
         <v>6</v>
@@ -1682,7 +1694,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B12">
         <v>43</v>
@@ -1690,7 +1702,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13">
         <v>6</v>
@@ -1704,7 +1716,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="A6:B8"/>
@@ -1716,54 +1728,59 @@
     <col min="2" max="2" width="14.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B2" s="8">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" s="8">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B4" s="8">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B5" s="8">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8"/>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6">
+        <v>67</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1795,7 +1812,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -1808,7 +1825,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>15</v>
@@ -1816,7 +1833,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -1824,7 +1841,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B5">
         <v>13</v>
@@ -1832,7 +1849,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>56</v>
@@ -1840,7 +1857,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B7">
         <v>15</v>
@@ -1848,7 +1865,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C8">
         <v>11</v>
@@ -1856,7 +1873,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C9">
         <v>34</v>
@@ -1871,7 +1888,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -1882,68 +1899,82 @@
     <col min="1" max="1" width="15.54296875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B7">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B8">
         <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1979,7 +2010,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -2018,7 +2049,7 @@
         <v>7</v>
       </c>
       <c r="C4">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <v>9</v>
@@ -2049,7 +2080,7 @@
         <v>11</v>
       </c>
       <c r="D6">
-        <v>14</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -2060,7 +2091,7 @@
         <v>7</v>
       </c>
       <c r="C7">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="D7">
         <v>12</v>

</xml_diff>